<commit_message>
Add explicit root to TemplateExcelFileGenerator
</commit_message>
<xml_diff>
--- a/fourPolar-io/src/test/resources/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/TemplateFourCamera.xlsx
+++ b/fourPolar-io/src/test/resources/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/TemplateFourCamera.xlsx
@@ -184,7 +184,10 @@
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.9"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Use assertThrown in ByExcelFinder
</commit_message>
<xml_diff>
--- a/fourPolar-io/src/test/resources/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/TemplateFourCamera.xlsx
+++ b/fourPolar-io/src/test/resources/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/TemplateFourCamera.xlsx
@@ -178,13 +178,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.9"/>
   </cols>
@@ -211,59 +211,59 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>